<commit_message>
Schema zu 65% fertiggestellt
</commit_message>
<xml_diff>
--- a/Dokumente/stueckliste.xlsx
+++ b/Dokumente/stueckliste.xlsx
@@ -19,11 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Stückliste!$A$3:$J$124</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Menge</t>
   </si>
@@ -60,13 +61,22 @@
   <si>
     <t>Bbc Lager</t>
   </si>
+  <si>
+    <t>2677095RL</t>
+  </si>
+  <si>
+    <t>Operationsverstärker</t>
+  </si>
+  <si>
+    <t>MOSFET 2N7002,215</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_ [$CHF-807]\ * #,##0.00_ ;_ [$CHF-807]\ * \-#,##0.00_ ;_ [$CHF-807]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$CHF-807]\ * #,##0.00_ ;_ [$CHF-807]\ * \-#,##0.00_ ;_ [$CHF-807]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -307,11 +317,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -625,7 +635,7 @@
   <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -644,10 +654,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="12"/>
       <c r="E1" s="12"/>
     </row>
@@ -688,10 +698,10 @@
       <c r="E3" s="20">
         <v>2</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>0.68</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <f>E3*F3</f>
         <v>1.36</v>
       </c>
@@ -710,36 +720,56 @@
       <c r="E4" s="21">
         <v>1</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>0.25</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <f t="shared" ref="G4:G67" si="0">E4*F4</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="21">
+        <v>4</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.43</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2315576</v>
+      </c>
+      <c r="E6" s="21">
+        <v>2</v>
+      </c>
+      <c r="F6" s="25">
+        <v>2.75E-2</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="0"/>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -748,8 +778,8 @@
       <c r="C7" s="8"/>
       <c r="D7" s="18"/>
       <c r="E7" s="21"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -760,8 +790,8 @@
       <c r="C8" s="8"/>
       <c r="D8" s="18"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26">
+      <c r="F8" s="25"/>
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -772,8 +802,8 @@
       <c r="C9" s="8"/>
       <c r="D9" s="18"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -784,8 +814,8 @@
       <c r="C10" s="8"/>
       <c r="D10" s="18"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26">
+      <c r="F10" s="25"/>
+      <c r="G10" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -796,8 +826,8 @@
       <c r="C11" s="8"/>
       <c r="D11" s="18"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -808,8 +838,8 @@
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26">
+      <c r="F12" s="25"/>
+      <c r="G12" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -820,8 +850,8 @@
       <c r="C13" s="8"/>
       <c r="D13" s="19"/>
       <c r="E13" s="21"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -832,8 +862,8 @@
       <c r="C14" s="8"/>
       <c r="D14" s="19"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -844,8 +874,8 @@
       <c r="C15" s="8"/>
       <c r="D15" s="19"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26">
+      <c r="F15" s="25"/>
+      <c r="G15" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -856,8 +886,8 @@
       <c r="C16" s="8"/>
       <c r="D16" s="19"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26">
+      <c r="F16" s="25"/>
+      <c r="G16" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -868,8 +898,8 @@
       <c r="C17" s="8"/>
       <c r="D17" s="19"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26">
+      <c r="F17" s="25"/>
+      <c r="G17" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -880,8 +910,8 @@
       <c r="C18" s="8"/>
       <c r="D18" s="19"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26">
+      <c r="F18" s="25"/>
+      <c r="G18" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -892,8 +922,8 @@
       <c r="C19" s="8"/>
       <c r="D19" s="19"/>
       <c r="E19" s="21"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26">
+      <c r="F19" s="25"/>
+      <c r="G19" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -904,8 +934,8 @@
       <c r="C20" s="8"/>
       <c r="D20" s="19"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26">
+      <c r="F20" s="25"/>
+      <c r="G20" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -916,8 +946,8 @@
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26">
+      <c r="F21" s="25"/>
+      <c r="G21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -928,8 +958,8 @@
       <c r="C22" s="8"/>
       <c r="D22" s="19"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26">
+      <c r="F22" s="25"/>
+      <c r="G22" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -940,8 +970,8 @@
       <c r="C23" s="8"/>
       <c r="D23" s="19"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26">
+      <c r="F23" s="25"/>
+      <c r="G23" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -952,8 +982,8 @@
       <c r="C24" s="8"/>
       <c r="D24" s="19"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26">
+      <c r="F24" s="25"/>
+      <c r="G24" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -964,8 +994,8 @@
       <c r="C25" s="8"/>
       <c r="D25" s="19"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26">
+      <c r="F25" s="25"/>
+      <c r="G25" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -976,8 +1006,8 @@
       <c r="C26" s="8"/>
       <c r="D26" s="19"/>
       <c r="E26" s="21"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26">
+      <c r="F26" s="25"/>
+      <c r="G26" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -988,8 +1018,8 @@
       <c r="C27" s="8"/>
       <c r="D27" s="19"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26">
+      <c r="F27" s="25"/>
+      <c r="G27" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1000,8 +1030,8 @@
       <c r="C28" s="8"/>
       <c r="D28" s="19"/>
       <c r="E28" s="21"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26">
+      <c r="F28" s="25"/>
+      <c r="G28" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1012,8 +1042,8 @@
       <c r="C29" s="8"/>
       <c r="D29" s="19"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26">
+      <c r="F29" s="25"/>
+      <c r="G29" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1024,8 +1054,8 @@
       <c r="C30" s="8"/>
       <c r="D30" s="19"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26">
+      <c r="F30" s="25"/>
+      <c r="G30" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1036,8 +1066,8 @@
       <c r="C31" s="8"/>
       <c r="D31" s="19"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26">
+      <c r="F31" s="25"/>
+      <c r="G31" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1048,8 +1078,8 @@
       <c r="C32" s="8"/>
       <c r="D32" s="19"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26">
+      <c r="F32" s="25"/>
+      <c r="G32" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1060,8 +1090,8 @@
       <c r="C33" s="8"/>
       <c r="D33" s="19"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26">
+      <c r="F33" s="25"/>
+      <c r="G33" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1072,8 +1102,8 @@
       <c r="C34" s="8"/>
       <c r="D34" s="19"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26">
+      <c r="F34" s="25"/>
+      <c r="G34" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1084,8 +1114,8 @@
       <c r="C35" s="15"/>
       <c r="D35" s="19"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26">
+      <c r="F35" s="25"/>
+      <c r="G35" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1096,8 +1126,8 @@
       <c r="C36" s="15"/>
       <c r="D36" s="19"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26">
+      <c r="F36" s="25"/>
+      <c r="G36" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1108,8 +1138,8 @@
       <c r="C37" s="15"/>
       <c r="D37" s="19"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26">
+      <c r="F37" s="25"/>
+      <c r="G37" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1120,8 +1150,8 @@
       <c r="C38" s="15"/>
       <c r="D38" s="19"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26">
+      <c r="F38" s="25"/>
+      <c r="G38" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1132,8 +1162,8 @@
       <c r="C39" s="15"/>
       <c r="D39" s="19"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26">
+      <c r="F39" s="25"/>
+      <c r="G39" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1144,8 +1174,8 @@
       <c r="C40" s="15"/>
       <c r="D40" s="19"/>
       <c r="E40" s="15"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26">
+      <c r="F40" s="25"/>
+      <c r="G40" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1156,8 +1186,8 @@
       <c r="C41" s="15"/>
       <c r="D41" s="19"/>
       <c r="E41" s="15"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26">
+      <c r="F41" s="25"/>
+      <c r="G41" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1168,8 +1198,8 @@
       <c r="C42" s="15"/>
       <c r="D42" s="19"/>
       <c r="E42" s="15"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26">
+      <c r="F42" s="25"/>
+      <c r="G42" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1180,8 +1210,8 @@
       <c r="C43" s="15"/>
       <c r="D43" s="19"/>
       <c r="E43" s="15"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26">
+      <c r="F43" s="25"/>
+      <c r="G43" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1192,8 +1222,8 @@
       <c r="C44" s="15"/>
       <c r="D44" s="19"/>
       <c r="E44" s="15"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26">
+      <c r="F44" s="25"/>
+      <c r="G44" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1204,8 +1234,8 @@
       <c r="C45" s="15"/>
       <c r="D45" s="19"/>
       <c r="E45" s="15"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26">
+      <c r="F45" s="25"/>
+      <c r="G45" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1216,8 +1246,8 @@
       <c r="C46" s="15"/>
       <c r="D46" s="19"/>
       <c r="E46" s="15"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26">
+      <c r="F46" s="25"/>
+      <c r="G46" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1228,8 +1258,8 @@
       <c r="C47" s="15"/>
       <c r="D47" s="19"/>
       <c r="E47" s="15"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26">
+      <c r="F47" s="25"/>
+      <c r="G47" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1240,8 +1270,8 @@
       <c r="C48" s="15"/>
       <c r="D48" s="19"/>
       <c r="E48" s="15"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26">
+      <c r="F48" s="25"/>
+      <c r="G48" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1252,8 +1282,8 @@
       <c r="C49" s="15"/>
       <c r="D49" s="19"/>
       <c r="E49" s="15"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26">
+      <c r="F49" s="25"/>
+      <c r="G49" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1264,8 +1294,8 @@
       <c r="C50" s="15"/>
       <c r="D50" s="19"/>
       <c r="E50" s="15"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26">
+      <c r="F50" s="25"/>
+      <c r="G50" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1276,8 +1306,8 @@
       <c r="C51" s="15"/>
       <c r="D51" s="19"/>
       <c r="E51" s="15"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26">
+      <c r="F51" s="25"/>
+      <c r="G51" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1288,8 +1318,8 @@
       <c r="C52" s="15"/>
       <c r="D52" s="19"/>
       <c r="E52" s="15"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26">
+      <c r="F52" s="25"/>
+      <c r="G52" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1301,8 +1331,8 @@
       <c r="C53" s="15"/>
       <c r="D53" s="19"/>
       <c r="E53" s="15"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26">
+      <c r="F53" s="25"/>
+      <c r="G53" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1313,8 +1343,8 @@
       <c r="C54" s="15"/>
       <c r="D54" s="19"/>
       <c r="E54" s="15"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26">
+      <c r="F54" s="25"/>
+      <c r="G54" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1325,8 +1355,8 @@
       <c r="C55" s="15"/>
       <c r="D55" s="19"/>
       <c r="E55" s="15"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26">
+      <c r="F55" s="25"/>
+      <c r="G55" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1337,8 +1367,8 @@
       <c r="C56" s="15"/>
       <c r="D56" s="19"/>
       <c r="E56" s="15"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26">
+      <c r="F56" s="25"/>
+      <c r="G56" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1349,8 +1379,8 @@
       <c r="C57" s="15"/>
       <c r="D57" s="19"/>
       <c r="E57" s="15"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26">
+      <c r="F57" s="25"/>
+      <c r="G57" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1361,8 +1391,8 @@
       <c r="C58" s="15"/>
       <c r="D58" s="19"/>
       <c r="E58" s="15"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26">
+      <c r="F58" s="25"/>
+      <c r="G58" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1373,8 +1403,8 @@
       <c r="C59" s="15"/>
       <c r="D59" s="19"/>
       <c r="E59" s="15"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26">
+      <c r="F59" s="25"/>
+      <c r="G59" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1385,8 +1415,8 @@
       <c r="C60" s="15"/>
       <c r="D60" s="19"/>
       <c r="E60" s="15"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26">
+      <c r="F60" s="25"/>
+      <c r="G60" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1397,8 +1427,8 @@
       <c r="C61" s="15"/>
       <c r="D61" s="19"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26">
+      <c r="F61" s="25"/>
+      <c r="G61" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1409,8 +1439,8 @@
       <c r="C62" s="15"/>
       <c r="D62" s="19"/>
       <c r="E62" s="15"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26">
+      <c r="F62" s="25"/>
+      <c r="G62" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1421,8 +1451,8 @@
       <c r="C63" s="15"/>
       <c r="D63" s="19"/>
       <c r="E63" s="15"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26">
+      <c r="F63" s="25"/>
+      <c r="G63" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1433,8 +1463,8 @@
       <c r="C64" s="15"/>
       <c r="D64" s="19"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="26">
+      <c r="F64" s="25"/>
+      <c r="G64" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1445,8 +1475,8 @@
       <c r="C65" s="15"/>
       <c r="D65" s="19"/>
       <c r="E65" s="15"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="26">
+      <c r="F65" s="25"/>
+      <c r="G65" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1457,8 +1487,8 @@
       <c r="C66" s="15"/>
       <c r="D66" s="19"/>
       <c r="E66" s="15"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26">
+      <c r="F66" s="25"/>
+      <c r="G66" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1469,8 +1499,8 @@
       <c r="C67" s="15"/>
       <c r="D67" s="19"/>
       <c r="E67" s="15"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="26">
+      <c r="F67" s="25"/>
+      <c r="G67" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1481,8 +1511,8 @@
       <c r="C68" s="15"/>
       <c r="D68" s="19"/>
       <c r="E68" s="15"/>
-      <c r="F68" s="26"/>
-      <c r="G68" s="26">
+      <c r="F68" s="25"/>
+      <c r="G68" s="25">
         <f t="shared" ref="G68:G114" si="1">E68*F68</f>
         <v>0</v>
       </c>
@@ -1493,8 +1523,8 @@
       <c r="C69" s="15"/>
       <c r="D69" s="19"/>
       <c r="E69" s="15"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26">
+      <c r="F69" s="25"/>
+      <c r="G69" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1505,8 +1535,8 @@
       <c r="C70" s="15"/>
       <c r="D70" s="19"/>
       <c r="E70" s="15"/>
-      <c r="F70" s="26"/>
-      <c r="G70" s="26">
+      <c r="F70" s="25"/>
+      <c r="G70" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1517,8 +1547,8 @@
       <c r="C71" s="15"/>
       <c r="D71" s="19"/>
       <c r="E71" s="15"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26">
+      <c r="F71" s="25"/>
+      <c r="G71" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1529,8 +1559,8 @@
       <c r="C72" s="15"/>
       <c r="D72" s="19"/>
       <c r="E72" s="15"/>
-      <c r="F72" s="26"/>
-      <c r="G72" s="26">
+      <c r="F72" s="25"/>
+      <c r="G72" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1541,8 +1571,8 @@
       <c r="C73" s="15"/>
       <c r="D73" s="19"/>
       <c r="E73" s="15"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26">
+      <c r="F73" s="25"/>
+      <c r="G73" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1553,8 +1583,8 @@
       <c r="C74" s="15"/>
       <c r="D74" s="19"/>
       <c r="E74" s="15"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="26">
+      <c r="F74" s="25"/>
+      <c r="G74" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1565,8 +1595,8 @@
       <c r="C75" s="15"/>
       <c r="D75" s="19"/>
       <c r="E75" s="15"/>
-      <c r="F75" s="26"/>
-      <c r="G75" s="26">
+      <c r="F75" s="25"/>
+      <c r="G75" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1577,8 +1607,8 @@
       <c r="C76" s="15"/>
       <c r="D76" s="19"/>
       <c r="E76" s="15"/>
-      <c r="F76" s="26"/>
-      <c r="G76" s="26">
+      <c r="F76" s="25"/>
+      <c r="G76" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1589,8 +1619,8 @@
       <c r="C77" s="15"/>
       <c r="D77" s="19"/>
       <c r="E77" s="15"/>
-      <c r="F77" s="26"/>
-      <c r="G77" s="26">
+      <c r="F77" s="25"/>
+      <c r="G77" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1601,8 +1631,8 @@
       <c r="C78" s="15"/>
       <c r="D78" s="19"/>
       <c r="E78" s="15"/>
-      <c r="F78" s="26"/>
-      <c r="G78" s="26">
+      <c r="F78" s="25"/>
+      <c r="G78" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1613,8 +1643,8 @@
       <c r="C79" s="15"/>
       <c r="D79" s="19"/>
       <c r="E79" s="15"/>
-      <c r="F79" s="26"/>
-      <c r="G79" s="26">
+      <c r="F79" s="25"/>
+      <c r="G79" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1625,8 +1655,8 @@
       <c r="C80" s="15"/>
       <c r="D80" s="19"/>
       <c r="E80" s="15"/>
-      <c r="F80" s="26"/>
-      <c r="G80" s="26">
+      <c r="F80" s="25"/>
+      <c r="G80" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1637,8 +1667,8 @@
       <c r="C81" s="15"/>
       <c r="D81" s="19"/>
       <c r="E81" s="15"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="26">
+      <c r="F81" s="25"/>
+      <c r="G81" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1649,8 +1679,8 @@
       <c r="C82" s="15"/>
       <c r="D82" s="19"/>
       <c r="E82" s="15"/>
-      <c r="F82" s="26"/>
-      <c r="G82" s="26">
+      <c r="F82" s="25"/>
+      <c r="G82" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1661,8 +1691,8 @@
       <c r="C83" s="15"/>
       <c r="D83" s="19"/>
       <c r="E83" s="15"/>
-      <c r="F83" s="26"/>
-      <c r="G83" s="26">
+      <c r="F83" s="25"/>
+      <c r="G83" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1673,8 +1703,8 @@
       <c r="C84" s="15"/>
       <c r="D84" s="19"/>
       <c r="E84" s="15"/>
-      <c r="F84" s="26"/>
-      <c r="G84" s="26">
+      <c r="F84" s="25"/>
+      <c r="G84" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1685,8 +1715,8 @@
       <c r="C85" s="15"/>
       <c r="D85" s="19"/>
       <c r="E85" s="15"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="26">
+      <c r="F85" s="25"/>
+      <c r="G85" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1697,8 +1727,8 @@
       <c r="C86" s="15"/>
       <c r="D86" s="19"/>
       <c r="E86" s="15"/>
-      <c r="F86" s="26"/>
-      <c r="G86" s="26">
+      <c r="F86" s="25"/>
+      <c r="G86" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1709,8 +1739,8 @@
       <c r="C87" s="15"/>
       <c r="D87" s="19"/>
       <c r="E87" s="15"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="26">
+      <c r="F87" s="25"/>
+      <c r="G87" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1721,8 +1751,8 @@
       <c r="C88" s="15"/>
       <c r="D88" s="19"/>
       <c r="E88" s="15"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="26">
+      <c r="F88" s="25"/>
+      <c r="G88" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1733,8 +1763,8 @@
       <c r="C89" s="15"/>
       <c r="D89" s="19"/>
       <c r="E89" s="15"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="26">
+      <c r="F89" s="25"/>
+      <c r="G89" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1745,8 +1775,8 @@
       <c r="C90" s="15"/>
       <c r="D90" s="19"/>
       <c r="E90" s="15"/>
-      <c r="F90" s="26"/>
-      <c r="G90" s="26">
+      <c r="F90" s="25"/>
+      <c r="G90" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1757,8 +1787,8 @@
       <c r="C91" s="15"/>
       <c r="D91" s="19"/>
       <c r="E91" s="15"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="26">
+      <c r="F91" s="25"/>
+      <c r="G91" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1769,8 +1799,8 @@
       <c r="C92" s="15"/>
       <c r="D92" s="19"/>
       <c r="E92" s="15"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="26">
+      <c r="F92" s="25"/>
+      <c r="G92" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1781,8 +1811,8 @@
       <c r="C93" s="15"/>
       <c r="D93" s="19"/>
       <c r="E93" s="15"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="26">
+      <c r="F93" s="25"/>
+      <c r="G93" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1793,8 +1823,8 @@
       <c r="C94" s="15"/>
       <c r="D94" s="19"/>
       <c r="E94" s="15"/>
-      <c r="F94" s="26"/>
-      <c r="G94" s="26">
+      <c r="F94" s="25"/>
+      <c r="G94" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1805,8 +1835,8 @@
       <c r="C95" s="15"/>
       <c r="D95" s="19"/>
       <c r="E95" s="15"/>
-      <c r="F95" s="26"/>
-      <c r="G95" s="26">
+      <c r="F95" s="25"/>
+      <c r="G95" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1817,8 +1847,8 @@
       <c r="C96" s="15"/>
       <c r="D96" s="19"/>
       <c r="E96" s="15"/>
-      <c r="F96" s="26"/>
-      <c r="G96" s="26">
+      <c r="F96" s="25"/>
+      <c r="G96" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1829,8 +1859,8 @@
       <c r="C97" s="15"/>
       <c r="D97" s="19"/>
       <c r="E97" s="15"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26">
+      <c r="F97" s="25"/>
+      <c r="G97" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1841,8 +1871,8 @@
       <c r="C98" s="15"/>
       <c r="D98" s="19"/>
       <c r="E98" s="15"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="26">
+      <c r="F98" s="25"/>
+      <c r="G98" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1853,8 +1883,8 @@
       <c r="C99" s="15"/>
       <c r="D99" s="19"/>
       <c r="E99" s="15"/>
-      <c r="F99" s="26"/>
-      <c r="G99" s="26">
+      <c r="F99" s="25"/>
+      <c r="G99" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1865,8 +1895,8 @@
       <c r="C100" s="15"/>
       <c r="D100" s="19"/>
       <c r="E100" s="15"/>
-      <c r="F100" s="26"/>
-      <c r="G100" s="26">
+      <c r="F100" s="25"/>
+      <c r="G100" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1877,8 +1907,8 @@
       <c r="C101" s="15"/>
       <c r="D101" s="19"/>
       <c r="E101" s="15"/>
-      <c r="F101" s="26"/>
-      <c r="G101" s="26">
+      <c r="F101" s="25"/>
+      <c r="G101" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1889,8 +1919,8 @@
       <c r="C102" s="15"/>
       <c r="D102" s="19"/>
       <c r="E102" s="15"/>
-      <c r="F102" s="26"/>
-      <c r="G102" s="26">
+      <c r="F102" s="25"/>
+      <c r="G102" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1901,8 +1931,8 @@
       <c r="C103" s="15"/>
       <c r="D103" s="19"/>
       <c r="E103" s="15"/>
-      <c r="F103" s="26"/>
-      <c r="G103" s="26">
+      <c r="F103" s="25"/>
+      <c r="G103" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1913,8 +1943,8 @@
       <c r="C104" s="15"/>
       <c r="D104" s="19"/>
       <c r="E104" s="15"/>
-      <c r="F104" s="26"/>
-      <c r="G104" s="26">
+      <c r="F104" s="25"/>
+      <c r="G104" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1925,8 +1955,8 @@
       <c r="C105" s="15"/>
       <c r="D105" s="19"/>
       <c r="E105" s="15"/>
-      <c r="F105" s="26"/>
-      <c r="G105" s="26">
+      <c r="F105" s="25"/>
+      <c r="G105" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1937,8 +1967,8 @@
       <c r="C106" s="15"/>
       <c r="D106" s="19"/>
       <c r="E106" s="15"/>
-      <c r="F106" s="26"/>
-      <c r="G106" s="26">
+      <c r="F106" s="25"/>
+      <c r="G106" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1949,8 +1979,8 @@
       <c r="C107" s="15"/>
       <c r="D107" s="19"/>
       <c r="E107" s="15"/>
-      <c r="F107" s="26"/>
-      <c r="G107" s="26">
+      <c r="F107" s="25"/>
+      <c r="G107" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1961,8 +1991,8 @@
       <c r="C108" s="15"/>
       <c r="D108" s="19"/>
       <c r="E108" s="15"/>
-      <c r="F108" s="26"/>
-      <c r="G108" s="26">
+      <c r="F108" s="25"/>
+      <c r="G108" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1973,8 +2003,8 @@
       <c r="C109" s="15"/>
       <c r="D109" s="19"/>
       <c r="E109" s="15"/>
-      <c r="F109" s="26"/>
-      <c r="G109" s="26">
+      <c r="F109" s="25"/>
+      <c r="G109" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1985,8 +2015,8 @@
       <c r="C110" s="15"/>
       <c r="D110" s="19"/>
       <c r="E110" s="15"/>
-      <c r="F110" s="26"/>
-      <c r="G110" s="26">
+      <c r="F110" s="25"/>
+      <c r="G110" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1997,8 +2027,8 @@
       <c r="C111" s="15"/>
       <c r="D111" s="19"/>
       <c r="E111" s="15"/>
-      <c r="F111" s="26"/>
-      <c r="G111" s="26">
+      <c r="F111" s="25"/>
+      <c r="G111" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2009,8 +2039,8 @@
       <c r="C112" s="15"/>
       <c r="D112" s="19"/>
       <c r="E112" s="15"/>
-      <c r="F112" s="26"/>
-      <c r="G112" s="26">
+      <c r="F112" s="25"/>
+      <c r="G112" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2021,8 +2051,8 @@
       <c r="C113" s="15"/>
       <c r="D113" s="19"/>
       <c r="E113" s="15"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="26">
+      <c r="F113" s="25"/>
+      <c r="G113" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2033,8 +2063,8 @@
       <c r="C114" s="15"/>
       <c r="D114" s="19"/>
       <c r="E114" s="15"/>
-      <c r="F114" s="26"/>
-      <c r="G114" s="26">
+      <c r="F114" s="25"/>
+      <c r="G114" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Schema bearbeitet; Sensor Simulation nun variabel
</commit_message>
<xml_diff>
--- a/Dokumente/stueckliste.xlsx
+++ b/Dokumente/stueckliste.xlsx
@@ -15,15 +15,15 @@
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Stückliste!$A$2:$F$113</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Stückliste!$A$3:$J$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Stückliste!$A$2:$F$111</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Stückliste!$A$3:$J$120</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>Menge</t>
   </si>
@@ -85,9 +85,6 @@
     <t>512-1N4148</t>
   </si>
   <si>
-    <t>Trimmpotentiometer</t>
-  </si>
-  <si>
     <t>DC/DC Wandler</t>
   </si>
   <si>
@@ -118,16 +115,214 @@
     <t xml:space="preserve">621-74LVC1G14W5-7 </t>
   </si>
   <si>
-    <t>Inverter</t>
-  </si>
-  <si>
-    <t>Schmitt-Trigger INV NAND SMD</t>
-  </si>
-  <si>
     <t>863-MBRS360T3G</t>
   </si>
   <si>
     <t>Schottkydiode</t>
+  </si>
+  <si>
+    <t>K5</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>K2,K3,K9</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>Q1,Q2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>K12</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>TP1-TP14</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>R3, R6</t>
+  </si>
+  <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>595-CD74HCT74E</t>
+  </si>
+  <si>
+    <t>Dual D Flip-Flop</t>
+  </si>
+  <si>
+    <t>579-MCP6004-I/P</t>
+  </si>
+  <si>
+    <t>OpAmp</t>
+  </si>
+  <si>
+    <t>K10, K13, K14</t>
+  </si>
+  <si>
+    <t>Balkenanzeige</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>859-LTA-1000G</t>
+  </si>
+  <si>
+    <t>595-UA78M05CDCYR</t>
+  </si>
+  <si>
+    <t>Linearer Spannungsreg. 5v 0.5A</t>
+  </si>
+  <si>
+    <t>K11</t>
+  </si>
+  <si>
+    <t>K6, K7, K8</t>
+  </si>
+  <si>
+    <t>80-C1206104K5RAC7867</t>
+  </si>
+  <si>
+    <t>Kondensator 100nF</t>
+  </si>
+  <si>
+    <t>C1, C5</t>
+  </si>
+  <si>
+    <t>Kondensator 1uF</t>
+  </si>
+  <si>
+    <t>80-C1206C105K4R</t>
+  </si>
+  <si>
+    <t>Trimmpotentiometer 100k</t>
+  </si>
+  <si>
+    <t>Trimmpotentiometer 2k</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Kondensator 330nF</t>
+  </si>
+  <si>
+    <t>C2-C4, C6, C7, C9, C13, C15-C20, C22</t>
+  </si>
+  <si>
+    <t>C11, C23</t>
+  </si>
+  <si>
+    <t>80-C1206C475K4PAC</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Kondensator 4.7uF</t>
+  </si>
+  <si>
+    <t>C12, C14</t>
+  </si>
+  <si>
+    <t>Kondensator 1.5uF</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Widerstand 39k</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-39K</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
+  </si>
+  <si>
+    <t>Widerstand 150</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-150R</t>
+  </si>
+  <si>
+    <t>Widerstand 1k</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-1K</t>
+  </si>
+  <si>
+    <t>Widerstand 1.5k</t>
+  </si>
+  <si>
+    <t>603-MFR-12FTF52-1K5</t>
+  </si>
+  <si>
+    <t>R13, R14</t>
+  </si>
+  <si>
+    <t>R9, R10, R11</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>Widerstand 10k</t>
+  </si>
+  <si>
+    <t>603-MFR-12FRF5210K</t>
+  </si>
+  <si>
+    <t>R17, R37</t>
+  </si>
+  <si>
+    <t>Widerstand 220</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-220R</t>
+  </si>
+  <si>
+    <t>R18-R20, R24, R28, R33-R37</t>
+  </si>
+  <si>
+    <t>Widerstand 470</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-470R</t>
+  </si>
+  <si>
+    <t>R21-R23, R25-R27, R29-R32</t>
+  </si>
+  <si>
+    <t>Widerstand 270</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-270R</t>
+  </si>
+  <si>
+    <t>Schmitt-Trigger NAND SMD</t>
+  </si>
+  <si>
+    <t>1G NOT Schmitt-Trigger</t>
   </si>
 </sst>
 </file>
@@ -302,7 +497,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -352,12 +547,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -370,9 +559,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -381,6 +567,45 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -691,10 +916,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -713,10 +938,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="12"/>
       <c r="E1" s="12"/>
     </row>
@@ -744,897 +969,1143 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="32">
         <v>9663762</v>
       </c>
-      <c r="E3" s="20">
-        <v>4</v>
-      </c>
-      <c r="F3" s="25">
+      <c r="E3" s="18">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22">
         <v>0.68</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <f>E3*F3</f>
-        <v>2.72</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="33">
         <v>1593464</v>
       </c>
-      <c r="E4" s="21">
-        <v>2</v>
-      </c>
-      <c r="F4" s="25">
+      <c r="E4" s="19">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22">
         <v>0.25</v>
       </c>
-      <c r="G4" s="25">
-        <f t="shared" ref="G4:G65" si="0">E4*F4</f>
-        <v>0.5</v>
+      <c r="G4" s="22">
+        <f t="shared" ref="G4:G63" si="0">E4*F4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="21">
-        <v>8</v>
-      </c>
-      <c r="F5" s="25">
+      <c r="E5" s="19">
+        <v>3</v>
+      </c>
+      <c r="F5" s="22">
         <v>0.43</v>
       </c>
-      <c r="G5" s="25">
-        <f t="shared" si="0"/>
-        <v>3.44</v>
+      <c r="G5" s="22">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="B6" s="8" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="21">
+      <c r="D6" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="19">
         <v>1</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>0.33800000000000002</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>0.33800000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>4</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>0.63100000000000001</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <f t="shared" si="0"/>
         <v>2.524</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="33">
         <v>2913817</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
         <v>2</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0.39700000000000002</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <f t="shared" si="0"/>
         <v>0.79400000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>2</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="22">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="22">
         <f t="shared" si="0"/>
         <v>0.184</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="33">
         <v>3259974</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <v>2</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="22">
         <v>3.03</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="22">
         <f t="shared" si="0"/>
         <v>6.06</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="B11" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="34">
         <v>1698982</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>1</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="22">
         <v>2.02</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="22">
         <f t="shared" si="0"/>
         <v>2.02</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="34">
         <v>1698983</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
         <v>1</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="22">
         <v>2.02</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="22">
         <f t="shared" si="0"/>
         <v>2.02</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="B13" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="21">
+      <c r="D13" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="19">
         <v>14</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <v>5.1799999999999999E-2</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <f t="shared" si="0"/>
         <v>0.72519999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="B14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="21">
+      <c r="D14" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="19">
         <v>1</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>0.34799999999999998</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <f t="shared" si="0"/>
         <v>0.34799999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="B15" s="8" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="21">
+      <c r="D15" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="19">
         <v>2</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <v>0.93</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="22">
         <f t="shared" si="0"/>
         <v>1.86</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="21">
+      <c r="D16" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="19">
         <v>3</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <v>0.26600000000000001</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="22">
         <f t="shared" si="0"/>
         <v>0.79800000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="B17" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="21">
+      <c r="D17" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="19">
         <v>2</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="22">
         <v>0.43</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="22">
         <f t="shared" si="0"/>
         <v>0.86</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="19">
+        <v>1</v>
+      </c>
+      <c r="F18" s="22">
+        <v>0.54</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A19" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="21">
+        <v>3</v>
+      </c>
+      <c r="F19" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="19">
+        <v>1</v>
+      </c>
+      <c r="F20" s="22">
+        <v>1.03</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="0"/>
+        <v>1.03</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="19">
+        <v>1</v>
+      </c>
+      <c r="F21" s="22">
+        <v>0.53</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="26" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="28">
+        <v>15</v>
+      </c>
+      <c r="F22" s="29">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G22" s="29">
+        <f t="shared" si="0"/>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="19">
+        <v>2</v>
+      </c>
+      <c r="F23" s="22">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="0"/>
+        <v>0.27400000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="34">
+        <v>1650900</v>
+      </c>
+      <c r="E24" s="19">
+        <v>2</v>
+      </c>
+      <c r="F24" s="22">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" si="0"/>
+        <v>0.27400000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="19">
+        <v>1</v>
+      </c>
+      <c r="F25" s="22">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="G25" s="22">
+        <f t="shared" si="0"/>
+        <v>0.30199999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="34">
+        <v>2820886</v>
+      </c>
+      <c r="E26" s="19">
+        <v>2</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="34">
+        <v>9354573</v>
+      </c>
+      <c r="E27" s="19">
+        <v>1</v>
+      </c>
+      <c r="F27" s="22">
+        <v>1.61</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="19">
+        <v>1</v>
+      </c>
+      <c r="F28" s="22">
+        <v>0.11</v>
+      </c>
+      <c r="G28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="19">
+        <v>2</v>
+      </c>
+      <c r="F29" s="22">
+        <v>0.11</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="19">
+        <v>3</v>
+      </c>
+      <c r="F30" s="22">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="0"/>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="15">
+        <v>2</v>
+      </c>
+      <c r="F31" s="22">
+        <v>0.129</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="0"/>
+        <v>0.25800000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="15">
+        <v>2</v>
+      </c>
+      <c r="F32" s="22">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="0"/>
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="15">
+        <v>2</v>
+      </c>
+      <c r="F33" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="25">
+        <v>9</v>
+      </c>
+      <c r="F34" s="30">
+        <v>0.11</v>
+      </c>
+      <c r="G34" s="30">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="31">
+        <v>10</v>
+      </c>
+      <c r="F35" s="30">
+        <v>0.11</v>
+      </c>
+      <c r="G35" s="30">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="19"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="22"/>
+      <c r="G36" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
-      <c r="D37" s="19"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="22"/>
+      <c r="G37" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="22"/>
+      <c r="G38" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
-      <c r="D39" s="19"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="22"/>
+      <c r="G39" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
-      <c r="D40" s="19"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="15"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="22"/>
+      <c r="G40" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
-      <c r="D41" s="19"/>
+      <c r="D41" s="17"/>
       <c r="E41" s="15"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="22"/>
+      <c r="G41" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
-      <c r="D42" s="19"/>
+      <c r="D42" s="17"/>
       <c r="E42" s="15"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="22"/>
+      <c r="G42" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
-      <c r="D43" s="19"/>
+      <c r="D43" s="17"/>
       <c r="E43" s="15"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="22"/>
+      <c r="G43" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
-      <c r="D44" s="19"/>
+      <c r="D44" s="17"/>
       <c r="E44" s="15"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="22"/>
+      <c r="G44" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
-      <c r="D45" s="19"/>
+      <c r="D45" s="17"/>
       <c r="E45" s="15"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="22"/>
+      <c r="G45" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
-      <c r="D46" s="19"/>
+      <c r="D46" s="17"/>
       <c r="E46" s="15"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="22"/>
+      <c r="G46" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
-      <c r="D47" s="19"/>
+      <c r="D47" s="17"/>
       <c r="E47" s="15"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="22"/>
+      <c r="G47" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="17"/>
       <c r="E48" s="15"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="22"/>
+      <c r="G48" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
-      <c r="D49" s="19"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="15"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="22"/>
+      <c r="G49" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
-      <c r="D50" s="19"/>
+      <c r="D50" s="17"/>
       <c r="E50" s="15"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J50" s="4"/>
-    </row>
-    <row r="51" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="22"/>
+      <c r="G50" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
-      <c r="D51" s="19"/>
+      <c r="D51" s="17"/>
       <c r="E51" s="15"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="22"/>
+      <c r="G51" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
-      <c r="D52" s="19"/>
+      <c r="D52" s="17"/>
       <c r="E52" s="15"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F52" s="22"/>
+      <c r="G52" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
-      <c r="D53" s="19"/>
+      <c r="D53" s="17"/>
       <c r="E53" s="15"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="22"/>
+      <c r="G53" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
-      <c r="D54" s="19"/>
+      <c r="D54" s="17"/>
       <c r="E54" s="15"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="22"/>
+      <c r="G54" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
-      <c r="D55" s="19"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="15"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="22"/>
+      <c r="G55" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
-      <c r="D56" s="19"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="15"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="22"/>
+      <c r="G56" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
-      <c r="D57" s="19"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="15"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F57" s="22"/>
+      <c r="G57" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
-      <c r="D58" s="19"/>
+      <c r="D58" s="17"/>
       <c r="E58" s="15"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="22"/>
+      <c r="G58" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
-      <c r="D59" s="19"/>
+      <c r="D59" s="17"/>
       <c r="E59" s="15"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F59" s="22"/>
+      <c r="G59" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
-      <c r="D60" s="19"/>
+      <c r="D60" s="17"/>
       <c r="E60" s="15"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="22"/>
+      <c r="G60" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="9"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
-      <c r="D61" s="19"/>
+      <c r="D61" s="17"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="22"/>
+      <c r="G61" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
-      <c r="D62" s="19"/>
+      <c r="D62" s="17"/>
       <c r="E62" s="15"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="22"/>
+      <c r="G62" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
-      <c r="D63" s="19"/>
+      <c r="D63" s="17"/>
       <c r="E63" s="15"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F63" s="22"/>
+      <c r="G63" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="9"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
-      <c r="D64" s="19"/>
+      <c r="D64" s="17"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25">
-        <f t="shared" si="0"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22">
+        <f t="shared" ref="G64:G110" si="1">E64*F64</f>
         <v>0</v>
       </c>
     </row>
@@ -1642,11 +2113,11 @@
       <c r="A65" s="9"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
-      <c r="D65" s="19"/>
+      <c r="D65" s="17"/>
       <c r="E65" s="15"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25">
-        <f t="shared" si="0"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1654,11 +2125,11 @@
       <c r="A66" s="9"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
-      <c r="D66" s="19"/>
+      <c r="D66" s="17"/>
       <c r="E66" s="15"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25">
-        <f t="shared" ref="G66:G112" si="1">E66*F66</f>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1666,10 +2137,10 @@
       <c r="A67" s="9"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
-      <c r="D67" s="19"/>
+      <c r="D67" s="17"/>
       <c r="E67" s="15"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25">
+      <c r="F67" s="22"/>
+      <c r="G67" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1678,10 +2149,10 @@
       <c r="A68" s="9"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
-      <c r="D68" s="19"/>
+      <c r="D68" s="17"/>
       <c r="E68" s="15"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25">
+      <c r="F68" s="22"/>
+      <c r="G68" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1690,10 +2161,10 @@
       <c r="A69" s="9"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
-      <c r="D69" s="19"/>
+      <c r="D69" s="17"/>
       <c r="E69" s="15"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25">
+      <c r="F69" s="22"/>
+      <c r="G69" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1702,10 +2173,10 @@
       <c r="A70" s="9"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
-      <c r="D70" s="19"/>
+      <c r="D70" s="17"/>
       <c r="E70" s="15"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25">
+      <c r="F70" s="22"/>
+      <c r="G70" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1714,10 +2185,10 @@
       <c r="A71" s="9"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
-      <c r="D71" s="19"/>
+      <c r="D71" s="17"/>
       <c r="E71" s="15"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25">
+      <c r="F71" s="22"/>
+      <c r="G71" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1726,10 +2197,10 @@
       <c r="A72" s="9"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
-      <c r="D72" s="19"/>
+      <c r="D72" s="17"/>
       <c r="E72" s="15"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25">
+      <c r="F72" s="22"/>
+      <c r="G72" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1738,10 +2209,10 @@
       <c r="A73" s="9"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
-      <c r="D73" s="19"/>
+      <c r="D73" s="17"/>
       <c r="E73" s="15"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25">
+      <c r="F73" s="22"/>
+      <c r="G73" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1750,10 +2221,10 @@
       <c r="A74" s="9"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
-      <c r="D74" s="19"/>
+      <c r="D74" s="17"/>
       <c r="E74" s="15"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25">
+      <c r="F74" s="22"/>
+      <c r="G74" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1762,10 +2233,10 @@
       <c r="A75" s="9"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
-      <c r="D75" s="19"/>
+      <c r="D75" s="17"/>
       <c r="E75" s="15"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25">
+      <c r="F75" s="22"/>
+      <c r="G75" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1774,10 +2245,10 @@
       <c r="A76" s="9"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
-      <c r="D76" s="19"/>
+      <c r="D76" s="17"/>
       <c r="E76" s="15"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25">
+      <c r="F76" s="22"/>
+      <c r="G76" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1786,10 +2257,10 @@
       <c r="A77" s="9"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
-      <c r="D77" s="19"/>
+      <c r="D77" s="17"/>
       <c r="E77" s="15"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25">
+      <c r="F77" s="22"/>
+      <c r="G77" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1798,10 +2269,10 @@
       <c r="A78" s="9"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
-      <c r="D78" s="19"/>
+      <c r="D78" s="17"/>
       <c r="E78" s="15"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25">
+      <c r="F78" s="22"/>
+      <c r="G78" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1810,10 +2281,10 @@
       <c r="A79" s="9"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
-      <c r="D79" s="19"/>
+      <c r="D79" s="17"/>
       <c r="E79" s="15"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25">
+      <c r="F79" s="22"/>
+      <c r="G79" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1822,10 +2293,10 @@
       <c r="A80" s="9"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
-      <c r="D80" s="19"/>
+      <c r="D80" s="17"/>
       <c r="E80" s="15"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25">
+      <c r="F80" s="22"/>
+      <c r="G80" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1834,10 +2305,10 @@
       <c r="A81" s="9"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
-      <c r="D81" s="19"/>
+      <c r="D81" s="17"/>
       <c r="E81" s="15"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25">
+      <c r="F81" s="22"/>
+      <c r="G81" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1846,10 +2317,10 @@
       <c r="A82" s="9"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
-      <c r="D82" s="19"/>
+      <c r="D82" s="17"/>
       <c r="E82" s="15"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25">
+      <c r="F82" s="22"/>
+      <c r="G82" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1858,10 +2329,10 @@
       <c r="A83" s="9"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
-      <c r="D83" s="19"/>
+      <c r="D83" s="17"/>
       <c r="E83" s="15"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="25">
+      <c r="F83" s="22"/>
+      <c r="G83" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1870,10 +2341,10 @@
       <c r="A84" s="9"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
-      <c r="D84" s="19"/>
+      <c r="D84" s="17"/>
       <c r="E84" s="15"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="25">
+      <c r="F84" s="22"/>
+      <c r="G84" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1882,10 +2353,10 @@
       <c r="A85" s="9"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
-      <c r="D85" s="19"/>
+      <c r="D85" s="17"/>
       <c r="E85" s="15"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="25">
+      <c r="F85" s="22"/>
+      <c r="G85" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1894,10 +2365,10 @@
       <c r="A86" s="9"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
-      <c r="D86" s="19"/>
+      <c r="D86" s="17"/>
       <c r="E86" s="15"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25">
+      <c r="F86" s="22"/>
+      <c r="G86" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1906,10 +2377,10 @@
       <c r="A87" s="9"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
-      <c r="D87" s="19"/>
+      <c r="D87" s="17"/>
       <c r="E87" s="15"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="25">
+      <c r="F87" s="22"/>
+      <c r="G87" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1918,10 +2389,10 @@
       <c r="A88" s="9"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
-      <c r="D88" s="19"/>
+      <c r="D88" s="17"/>
       <c r="E88" s="15"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="25">
+      <c r="F88" s="22"/>
+      <c r="G88" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1930,10 +2401,10 @@
       <c r="A89" s="9"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
-      <c r="D89" s="19"/>
+      <c r="D89" s="17"/>
       <c r="E89" s="15"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="25">
+      <c r="F89" s="22"/>
+      <c r="G89" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1942,10 +2413,10 @@
       <c r="A90" s="9"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
-      <c r="D90" s="19"/>
+      <c r="D90" s="17"/>
       <c r="E90" s="15"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25">
+      <c r="F90" s="22"/>
+      <c r="G90" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1954,10 +2425,10 @@
       <c r="A91" s="9"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
-      <c r="D91" s="19"/>
+      <c r="D91" s="17"/>
       <c r="E91" s="15"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25">
+      <c r="F91" s="22"/>
+      <c r="G91" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1966,10 +2437,10 @@
       <c r="A92" s="9"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
-      <c r="D92" s="19"/>
+      <c r="D92" s="17"/>
       <c r="E92" s="15"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25">
+      <c r="F92" s="22"/>
+      <c r="G92" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1978,10 +2449,10 @@
       <c r="A93" s="9"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
-      <c r="D93" s="19"/>
+      <c r="D93" s="17"/>
       <c r="E93" s="15"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="25">
+      <c r="F93" s="22"/>
+      <c r="G93" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1990,10 +2461,10 @@
       <c r="A94" s="9"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
-      <c r="D94" s="19"/>
+      <c r="D94" s="17"/>
       <c r="E94" s="15"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25">
+      <c r="F94" s="22"/>
+      <c r="G94" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2002,10 +2473,10 @@
       <c r="A95" s="9"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
-      <c r="D95" s="19"/>
+      <c r="D95" s="17"/>
       <c r="E95" s="15"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="25">
+      <c r="F95" s="22"/>
+      <c r="G95" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2014,10 +2485,10 @@
       <c r="A96" s="9"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
-      <c r="D96" s="19"/>
+      <c r="D96" s="17"/>
       <c r="E96" s="15"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="25">
+      <c r="F96" s="22"/>
+      <c r="G96" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2026,10 +2497,10 @@
       <c r="A97" s="9"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
-      <c r="D97" s="19"/>
+      <c r="D97" s="17"/>
       <c r="E97" s="15"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="25">
+      <c r="F97" s="22"/>
+      <c r="G97" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2038,10 +2509,10 @@
       <c r="A98" s="9"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
-      <c r="D98" s="19"/>
+      <c r="D98" s="17"/>
       <c r="E98" s="15"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="25">
+      <c r="F98" s="22"/>
+      <c r="G98" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2050,10 +2521,10 @@
       <c r="A99" s="9"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
-      <c r="D99" s="19"/>
+      <c r="D99" s="17"/>
       <c r="E99" s="15"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="25">
+      <c r="F99" s="22"/>
+      <c r="G99" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2062,10 +2533,10 @@
       <c r="A100" s="9"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
-      <c r="D100" s="19"/>
+      <c r="D100" s="17"/>
       <c r="E100" s="15"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25">
+      <c r="F100" s="22"/>
+      <c r="G100" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2074,10 +2545,10 @@
       <c r="A101" s="9"/>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
-      <c r="D101" s="19"/>
+      <c r="D101" s="17"/>
       <c r="E101" s="15"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="25">
+      <c r="F101" s="22"/>
+      <c r="G101" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2086,10 +2557,10 @@
       <c r="A102" s="9"/>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
-      <c r="D102" s="19"/>
+      <c r="D102" s="17"/>
       <c r="E102" s="15"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25">
+      <c r="F102" s="22"/>
+      <c r="G102" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2098,10 +2569,10 @@
       <c r="A103" s="9"/>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>
-      <c r="D103" s="19"/>
+      <c r="D103" s="17"/>
       <c r="E103" s="15"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="25">
+      <c r="F103" s="22"/>
+      <c r="G103" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2110,10 +2581,10 @@
       <c r="A104" s="9"/>
       <c r="B104" s="15"/>
       <c r="C104" s="15"/>
-      <c r="D104" s="19"/>
+      <c r="D104" s="17"/>
       <c r="E104" s="15"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25">
+      <c r="F104" s="22"/>
+      <c r="G104" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2122,10 +2593,10 @@
       <c r="A105" s="9"/>
       <c r="B105" s="15"/>
       <c r="C105" s="15"/>
-      <c r="D105" s="19"/>
+      <c r="D105" s="17"/>
       <c r="E105" s="15"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="25">
+      <c r="F105" s="22"/>
+      <c r="G105" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2134,10 +2605,10 @@
       <c r="A106" s="9"/>
       <c r="B106" s="15"/>
       <c r="C106" s="15"/>
-      <c r="D106" s="19"/>
+      <c r="D106" s="17"/>
       <c r="E106" s="15"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="25">
+      <c r="F106" s="22"/>
+      <c r="G106" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2146,10 +2617,10 @@
       <c r="A107" s="9"/>
       <c r="B107" s="15"/>
       <c r="C107" s="15"/>
-      <c r="D107" s="19"/>
+      <c r="D107" s="17"/>
       <c r="E107" s="15"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="25">
+      <c r="F107" s="22"/>
+      <c r="G107" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2158,10 +2629,10 @@
       <c r="A108" s="9"/>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
-      <c r="D108" s="19"/>
+      <c r="D108" s="17"/>
       <c r="E108" s="15"/>
-      <c r="F108" s="25"/>
-      <c r="G108" s="25">
+      <c r="F108" s="22"/>
+      <c r="G108" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2170,49 +2641,43 @@
       <c r="A109" s="9"/>
       <c r="B109" s="15"/>
       <c r="C109" s="15"/>
-      <c r="D109" s="19"/>
+      <c r="D109" s="17"/>
       <c r="E109" s="15"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F109" s="22"/>
+      <c r="G109" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="9"/>
       <c r="B110" s="15"/>
       <c r="C110" s="15"/>
-      <c r="D110" s="19"/>
+      <c r="D110" s="17"/>
       <c r="E110" s="15"/>
-      <c r="F110" s="25"/>
-      <c r="G110" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="9"/>
-      <c r="B111" s="15"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="15"/>
-      <c r="F111" s="25"/>
-      <c r="G111" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="6"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="9"/>
-      <c r="B112" s="15"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="25"/>
-      <c r="G112" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A112" s="6"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
@@ -2233,22 +2698,10 @@
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="6"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
+      <c r="D115" s="5"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="6"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
+      <c r="D116" s="5"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D117" s="5"/>
@@ -2256,14 +2709,8 @@
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D118" s="5"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D119" s="5"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D120" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:F113"/>
+  <autoFilter ref="A2:F111"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>

</xml_diff>